<commit_message>
added a backup of the database
</commit_message>
<xml_diff>
--- a/Databases/MobiedockDataFiles/Excel Tables:Other Docs/ErrorLog.xlsx
+++ b/Databases/MobiedockDataFiles/Excel Tables:Other Docs/ErrorLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bendavis/Documents/solar-scooter-project/Databases/MobiedockDataFiles/Excel Tables:Other Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F478B355-C5CA-0644-826D-092707920FB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFB6731-B701-3742-8236-F377FD3D5C9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12860" windowHeight="15540" xr2:uid="{B83D6F8C-48A8-2047-A231-66282858B479}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>E4</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>S2</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R1</t>
   </si>
 </sst>
 </file>
@@ -395,42 +401,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC80538-05E9-064A-BACF-10A5B1AB0ABA}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1">
         <v>43434</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
         <v>43435</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>